<commit_message>
xóa dòng Tổng ở cuối
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Temp_LichSuMua_ThanhToan_TichLuy_ofKhachHang.xlsx
+++ b/banhang24/Template/ExportExcel/Temp_LichSuMua_ThanhToan_TichLuy_ofKhachHang.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT Source Code\KangJinDemo\banhang24\Template\ExportExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SSOFT\KangjinDemo2\KangJinDemo\banhang24\Template\ExportExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9600"/>
   </bookViews>
   <sheets>
     <sheet name="LichSuBanHang" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Mã khách hàng:</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>Tổng cộng</t>
-  </si>
-  <si>
-    <t>Tổng cộng:</t>
   </si>
   <si>
     <t>Người tạo</t>
@@ -142,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -165,48 +162,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -269,9 +229,6 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -284,15 +241,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -301,12 +249,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -591,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,13 +550,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="A1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
@@ -639,13 +581,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,21 +723,43 @@
       <c r="D25" s="21"/>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="22">
-        <f xml:space="preserve"> SUM(D$7:D25)</f>
-        <v>0</v>
-      </c>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="21"/>
       <c r="E26" s="9"/>
     </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A26:C26"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -805,10 +769,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,12 +786,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="A1" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -843,7 +807,7 @@
     </row>
     <row r="6" spans="1:5" s="14" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>3</v>
@@ -855,7 +819,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -991,21 +955,8 @@
       <c r="D25" s="21"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="22">
-        <f xml:space="preserve"> SUM(D$7:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A26:C26"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1015,10 +966,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1026,19 +977,19 @@
     <col min="1" max="1" width="17.140625" style="8" customWidth="1"/>
     <col min="2" max="2" width="21.28515625" style="17" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="22" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" style="19" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
+      <c r="A1" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1052,171 +1003,158 @@
       </c>
       <c r="B4" s="18"/>
     </row>
-    <row r="6" spans="1:5" s="26" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:5" s="25" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="E6" s="20" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="16"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="24"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="21"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="16"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="24"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="16"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="24"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="24"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="16"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="24"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="16"/>
       <c r="C12" s="4"/>
-      <c r="D12" s="24"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="16"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="24"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="21"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="16"/>
       <c r="C14" s="4"/>
-      <c r="D14" s="24"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="16"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="24"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="21"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="16"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="24"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="21"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="16"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="24"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="16"/>
       <c r="C18" s="4"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="16"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="24"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="16"/>
       <c r="C20" s="4"/>
-      <c r="D20" s="24"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="16"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="24"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="21"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="16"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="24"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="16"/>
       <c r="C23" s="4"/>
-      <c r="D23" s="24"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="16"/>
       <c r="C24" s="4"/>
-      <c r="D24" s="24"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="16"/>
       <c r="C25" s="4"/>
-      <c r="D25" s="24"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="21"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="22">
-        <f>SUM(D$7:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="22"/>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A26:C26"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1226,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1244,14 +1182,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
+      <c r="A1" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -1267,22 +1205,22 @@
     </row>
     <row r="6" spans="1:6" s="14" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>14</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1437,25 +1375,48 @@
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
     </row>
-    <row r="26" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="22">
-        <f xml:space="preserve"> SUM(D$7:D25)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="22">
-        <f xml:space="preserve"> SUM(E$7:E25)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="22"/>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A26:C26"/>
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>